<commit_message>
Slowly implementing computation examples.
</commit_message>
<xml_diff>
--- a/data/DeLaatFig5.xlsx
+++ b/data/DeLaatFig5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/Entiteiten/Hygea/2022-AGT/jupyter/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74F6A77B-A185-C244-84E0-C6805F7E2066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63853A8-B0C7-BA49-A365-327C831B221B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FB42C4C5-D1A7-9946-84C8-9F1E561AD6AB}"/>
   </bookViews>
@@ -184,444 +184,684 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$72</c:f>
+              <c:f>Sheet1!$A$2:$A$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="111"/>
                 <c:pt idx="0">
-                  <c:v>1.0095815654458999</c:v>
+                  <c:v>1.0841509701135801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.25159749693963</c:v>
+                  <c:v>1.0148120865928001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5361679002366599</c:v>
+                  <c:v>1.3304026190881399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8854190621678399</c:v>
+                  <c:v>1.6331948483645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.31418815353382</c:v>
+                  <c:v>2.0050838767606698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8401515660405598</c:v>
+                  <c:v>2.4969099235247199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4850201812902899</c:v>
+                  <c:v>3.0209128793669602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2752710145950203</c:v>
+                  <c:v>3.5983252571833901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.2449478210778899</c:v>
+                  <c:v>3.8464593649532199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.4346286124465797</c:v>
+                  <c:v>4.7198374164153396</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.8686619466667098</c:v>
+                  <c:v>5.7900614802659103</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.2107221251120901</c:v>
+                  <c:v>7.1014135015007103</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.086540162263701</c:v>
+                  <c:v>8.7621572729251902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.221029926230001</c:v>
+                  <c:v>9.1447771622803202</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.674659992076499</c:v>
+                  <c:v>10.4469455604497</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.1367203381796</c:v>
+                  <c:v>12.512343717956799</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.714399637650999</c:v>
+                  <c:v>13.9989445875703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22.541189718014799</c:v>
+                  <c:v>16.0173832403663</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25.3491937621916</c:v>
+                  <c:v>18.560655288486</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.954096173884299</c:v>
+                  <c:v>21.262252697184699</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.801427277065098</c:v>
+                  <c:v>23.529018070784598</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31.9381413554689</c:v>
+                  <c:v>25.871948633781301</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>33.701512883846597</c:v>
+                  <c:v>29.072804382953301</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.109098894319601</c:v>
+                  <c:v>31.163733325723101</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>38.606005256630603</c:v>
+                  <c:v>32.326347885670899</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41.527836641609703</c:v>
+                  <c:v>33.654750654514302</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>43.887672944765001</c:v>
+                  <c:v>36.1977058896437</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>47.001826950049796</c:v>
+                  <c:v>38.686720807110902</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>49.267796913246798</c:v>
+                  <c:v>41.599527334404002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54.477482995020203</c:v>
+                  <c:v>43.613893514893697</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>56.462796987803998</c:v>
+                  <c:v>46.2132871444987</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>60.8687897231612</c:v>
+                  <c:v>48.5047571661094</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>63.268847012837703</c:v>
+                  <c:v>48.2353987753513</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>64.940211589056005</c:v>
+                  <c:v>54.494067774064099</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>67.304352800524697</c:v>
+                  <c:v>56.757968002344498</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>71.051095493541098</c:v>
+                  <c:v>58.675022645108903</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>75.677116702132494</c:v>
+                  <c:v>61.040589793358897</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76.986691668114901</c:v>
+                  <c:v>63.846555736272101</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>85.477650006688606</c:v>
+                  <c:v>68.265341107002996</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>91.994501206134501</c:v>
+                  <c:v>66.246967750450395</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>94.995048345824998</c:v>
+                  <c:v>70.322036375775994</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>96.762959024491096</c:v>
+                  <c:v>72.393505542767997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>113.70095782057599</c:v>
+                  <c:v>78.051031204444399</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>136.04434132363201</c:v>
+                  <c:v>81.358143409159098</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>161.55212855826801</c:v>
+                  <c:v>81.496142530730793</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>182.12625823331899</c:v>
+                  <c:v>80.896064482197104</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>203.41223625609001</c:v>
+                  <c:v>82.8777453045101</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>235.22511807625901</c:v>
+                  <c:v>84.276648023166999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>269.85958334609302</c:v>
+                  <c:v>86.643613588577693</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>318.39737104644303</c:v>
+                  <c:v>86.496546609847698</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>365.079639120965</c:v>
+                  <c:v>86.346085833071001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>419.80451298070199</c:v>
+                  <c:v>87.5875386177472</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>485.78503071000301</c:v>
+                  <c:v>90.030859637044699</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>561.79084593225696</c:v>
+                  <c:v>87.003790957947203</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>655.79953646961201</c:v>
+                  <c:v>91.209509638601304</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>766.59880799493601</c:v>
+                  <c:v>97.045815206610897</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>888.86973182429904</c:v>
+                  <c:v>88.349552566529795</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1001.2753794142</c:v>
+                  <c:v>95.123924984559594</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1204.6832128313499</c:v>
+                  <c:v>94.865130271119398</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1366.8453975648699</c:v>
+                  <c:v>98.271826379985697</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1580.5658206133801</c:v>
+                  <c:v>99.341778561223904</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1800.1104189345899</c:v>
+                  <c:v>110.57609466959001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2150.68205073436</c:v>
+                  <c:v>108.531296147633</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2508.4453869231302</c:v>
+                  <c:v>109.047934348423</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2928.79658559769</c:v>
+                  <c:v>122.939263148932</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3473.0750334785998</c:v>
+                  <c:v>141.33065011476401</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4147.4340533139302</c:v>
+                  <c:v>159.07563654518299</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4788.7301113032199</c:v>
+                  <c:v>184.26929824817199</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5569.6668085525998</c:v>
+                  <c:v>216.123753975559</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6518.0657198635299</c:v>
+                  <c:v>250.49950480627101</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7950.1610284071303</c:v>
+                  <c:v>250.905443557729</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>303.07743952549203</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>339.49576030262602</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>395.62402844562899</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>370.87013628711298</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>461.78579671032497</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>538.924100799793</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>627.21338137340899</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>734.10782031617305</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>846.897692369315</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>951.26593595622501</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1098.9062216530699</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1201.026131549</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1398.6619285531301</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1643.5524190533999</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1813.3746760596</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2131.7633579895</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2482.9754241734599</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2887.5722612120899</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3423.3166876266901</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4086.9464512763898</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4717.65946368408</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5485.7135259003899</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6418.2891617462601</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>7299.0485756717999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>7947.6124466579804</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9078.6007991418501</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9459.4431575939907</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10050.6248573665</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10556.2744715643</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11736.963222706399</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>13106.7560347014</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>15311.3134042727</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>17802.546001398201</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>20633.850060215202</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>23992.0141466803</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>28144.987186210001</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>32726.027316800701</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>36081.3550923855</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>38151.687840322702</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>44237.405673204601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$72</c:f>
+              <c:f>Sheet1!$B$2:$B$112</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="111"/>
                 <c:pt idx="0">
-                  <c:v>76.560722838756107</c:v>
+                  <c:v>78.0289513918474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75.859482620915202</c:v>
+                  <c:v>70.431663956706899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>73.369980518217702</c:v>
+                  <c:v>72.310206630739302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.831689344323607</c:v>
+                  <c:v>70.357539305263003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68.949923167216298</c:v>
+                  <c:v>69.280918687568004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.894119770480003</c:v>
+                  <c:v>65.648041480345</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61.0900625862404</c:v>
+                  <c:v>63.5609222325388</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.3887643365901</c:v>
+                  <c:v>65.071934949524405</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48.780375507067397</c:v>
+                  <c:v>55.811862965879399</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43.830902933628202</c:v>
+                  <c:v>51.295104598775502</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.046191917891299</c:v>
+                  <c:v>45.6086895881432</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.7863024997304</c:v>
+                  <c:v>39.412905286025399</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25.445326306123899</c:v>
+                  <c:v>33.079029576034401</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.131214107971701</c:v>
+                  <c:v>44.766931689715001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.4906121668234</c:v>
+                  <c:v>26.6612902057627</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.403029956667201</c:v>
+                  <c:v>21.6039587390826</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.1047685567921</c:v>
+                  <c:v>17.604522871673002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.3869796419968594</c:v>
+                  <c:v>14.4090697526594</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.3121890520666097</c:v>
+                  <c:v>11.212771153202899</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.82464428089542</c:v>
+                  <c:v>8.7291844023060108</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9120280447992202</c:v>
+                  <c:v>6.5849134161323901</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.2112078285354699</c:v>
+                  <c:v>5.47652739045009</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.60907253014076</c:v>
+                  <c:v>4.4292995696422199</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.0893236627337899</c:v>
+                  <c:v>3.28477154219238</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.6285273619312099</c:v>
+                  <c:v>5.8424510213520398</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2439783977274299</c:v>
+                  <c:v>2.53303250117209</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.91311254106637496</c:v>
+                  <c:v>2.0008160389890501</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.68584893320657903</c:v>
+                  <c:v>1.55563377093876</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.49329822216580199</c:v>
+                  <c:v>1.1893248134030301</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.34014980623567298</c:v>
+                  <c:v>0.89250856625370201</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.25634284782254302</c:v>
+                  <c:v>0.73494865583824998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.18218110942808899</c:v>
+                  <c:v>0.46831213076936401</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.121042157780367</c:v>
+                  <c:v>0.604398687952172</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.8310602348460096E-2</c:v>
+                  <c:v>0.32494650256065399</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.8446627050070499E-2</c:v>
+                  <c:v>0.24617415358535499</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.1085742307097302E-2</c:v>
+                  <c:v>0.44443288556222599</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.5553435166939901E-2</c:v>
+                  <c:v>0.17473151875764001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.7748208041007999E-2</c:v>
+                  <c:v>0.117323914081486</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1330278663637601E-2</c:v>
+                  <c:v>8.5775569736564306E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.8939678652236401E-3</c:v>
+                  <c:v>0.44925200570586299</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.59983192549371E-3</c:v>
+                  <c:v>6.3408360487477694E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.2925223368789099E-3</c:v>
+                  <c:v>4.8351530876371299E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.04609218064063E-3</c:v>
+                  <c:v>3.6640873828206903E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.9639939235247E-4</c:v>
+                  <c:v>2.55262068377799E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.8304332030692995E-4</c:v>
+                  <c:v>2.7112226828618301E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.6894811732143703E-4</c:v>
+                  <c:v>1.8989171866098001E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.7614579180989899E-4</c:v>
+                  <c:v>1.51663326967354E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.0040777950631999E-4</c:v>
+                  <c:v>1.1474200878648901E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.35789198278995E-4</c:v>
+                  <c:v>9.9672381548971595E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.9233740156918101E-4</c:v>
+                  <c:v>7.9785609546122294E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.5097291974243201E-4</c:v>
+                  <c:v>6.3514624165424499E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.20692836258391E-4</c:v>
+                  <c:v>8.7276918971913205E-3</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>9.6382205947926695E-5</c:v>
+                  <c:v>6.18393766969176E-3</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.7685492186039997E-5</c:v>
+                  <c:v>5.0555110252974399E-2</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>6.1429989804976003E-5</c:v>
+                  <c:v>4.7180917555339798E-3</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>4.86741543837627E-5</c:v>
+                  <c:v>3.5347882569146498E-2</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>3.8940039623371102E-5</c:v>
+                  <c:v>3.2763520924367198E-2</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>3.0628958137867202E-5</c:v>
+                  <c:v>3.49192757902548E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>2.4835223316413401E-5</c:v>
+                  <c:v>1.80038975524059E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>1.9762926960883999E-5</c:v>
+                  <c:v>1.37821155828402E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>1.5702406017156599E-5</c:v>
+                  <c:v>2.5206641425463399E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>1.38442756359114E-5</c:v>
+                  <c:v>1.0810997293002401E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>9.9913835185145703E-6</c:v>
+                  <c:v>3.4853114241845798E-2</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>7.8082334896095392E-6</c:v>
+                  <c:v>1.6594236197382301E-3</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>6.1169326693710102E-6</c:v>
+                  <c:v>8.1914637196573098E-4</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>4.77977201231022E-6</c:v>
+                  <c:v>6.4075855074308195E-4</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>3.67233817295874E-6</c:v>
+                  <c:v>5.1399535178800297E-4</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>2.92129795750396E-6</c:v>
+                  <c:v>4.1900055355496201E-4</c:v>
                 </c:pt>
                 <c:pt idx="68" formatCode="0.00E+00">
-                  <c:v>2.3276475615925101E-6</c:v>
+                  <c:v>3.2644129184313198E-4</c:v>
                 </c:pt>
                 <c:pt idx="69" formatCode="0.00E+00">
-                  <c:v>1.83474763079065E-6</c:v>
+                  <c:v>2.5581057894239102E-4</c:v>
                 </c:pt>
                 <c:pt idx="70" formatCode="0.00E+00">
-                  <c:v>1.3081622749432499E-6</c:v>
+                  <c:v>2.1042563118213101E-4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.0076997405015201E-4</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.7256392386403899E-4</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.2678615838915901E-4</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.8231453403693199E-4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>9.8797488401080005E-5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.7961525529283605E-5</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.1822950516881098E-5</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.8408666217356403E-5</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.0382334007166997E-5</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.0406916100686101E-5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.6400590671502999E-5</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.21750249519291E-5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.67807455661695E-5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.44636844949744E-5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.19210692061932E-5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9.4892639888764302E-6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.4559063534511701E-6</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.8510619605561803E-6</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.5633272207078901E-6</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.5061097179644399E-6</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.7802954529325599E-6</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.21282709925747E-6</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.7444233816782701E-6</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.2781540600331E-6</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.3349797999698301E-6</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.1248959165915299E-6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.6317509882533701E-6</c:v>
+                </c:pt>
+                <c:pt idx="98" formatCode="0.00E+00">
+                  <c:v>7.8568298476819795E-7</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.21422512006453E-6</c:v>
+                </c:pt>
+                <c:pt idx="100" formatCode="0.00E+00">
+                  <c:v>7.1204060224130796E-7</c:v>
+                </c:pt>
+                <c:pt idx="101" formatCode="0.00E+00">
+                  <c:v>5.7904533682010705E-7</c:v>
+                </c:pt>
+                <c:pt idx="102" formatCode="0.00E+00">
+                  <c:v>4.6204223536916198E-7</c:v>
+                </c:pt>
+                <c:pt idx="103" formatCode="0.00E+00">
+                  <c:v>3.6367121301650998E-7</c:v>
+                </c:pt>
+                <c:pt idx="104" formatCode="0.00E+00">
+                  <c:v>2.9135090582297602E-7</c:v>
+                </c:pt>
+                <c:pt idx="105" formatCode="0.00E+00">
+                  <c:v>2.30483700714755E-7</c:v>
+                </c:pt>
+                <c:pt idx="106" formatCode="0.00E+00">
+                  <c:v>1.8422259950331399E-7</c:v>
+                </c:pt>
+                <c:pt idx="107" formatCode="0.00E+00">
+                  <c:v>1.45990928302693E-7</c:v>
+                </c:pt>
+                <c:pt idx="108" formatCode="0.00E+00">
+                  <c:v>9.6489569562621105E-8</c:v>
+                </c:pt>
+                <c:pt idx="109" formatCode="0.00E+00">
+                  <c:v>1.2021627605778299E-7</c:v>
+                </c:pt>
+                <c:pt idx="110" formatCode="0.00E+00">
+                  <c:v>1.01614257109751E-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1736,10 +1976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C93435C-E824-2542-9F14-49197ACEFEBA}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1754,570 +1994,890 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1.0095815654458999</v>
+        <v>1.0841509701135801</v>
       </c>
       <c r="B2">
-        <v>76.560722838756107</v>
+        <v>78.0289513918474</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.25159749693963</v>
+        <v>1.0148120865928001</v>
       </c>
       <c r="B3">
-        <v>75.859482620915202</v>
+        <v>70.431663956706899</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.5361679002366599</v>
+        <v>1.3304026190881399</v>
       </c>
       <c r="B4">
-        <v>73.369980518217702</v>
+        <v>72.310206630739302</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.8854190621678399</v>
+        <v>1.6331948483645</v>
       </c>
       <c r="B5">
-        <v>70.831689344323607</v>
+        <v>70.357539305263003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2.31418815353382</v>
+        <v>2.0050838767606698</v>
       </c>
       <c r="B6">
-        <v>68.949923167216298</v>
+        <v>69.280918687568004</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2.8401515660405598</v>
+        <v>2.4969099235247199</v>
       </c>
       <c r="B7">
-        <v>65.894119770480003</v>
+        <v>65.648041480345</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3.4850201812902899</v>
+        <v>3.0209128793669602</v>
       </c>
       <c r="B8">
-        <v>61.0900625862404</v>
+        <v>63.5609222325388</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4.2752710145950203</v>
+        <v>3.5983252571833901</v>
       </c>
       <c r="B9">
-        <v>54.3887643365901</v>
+        <v>65.071934949524405</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>5.2449478210778899</v>
+        <v>3.8464593649532199</v>
       </c>
       <c r="B10">
-        <v>48.780375507067397</v>
+        <v>55.811862965879399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>6.4346286124465797</v>
+        <v>4.7198374164153396</v>
       </c>
       <c r="B11">
-        <v>43.830902933628202</v>
+        <v>51.295104598775502</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>7.8686619466667098</v>
+        <v>5.7900614802659103</v>
       </c>
       <c r="B12">
-        <v>37.046191917891299</v>
+        <v>45.6086895881432</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>9.2107221251120901</v>
+        <v>7.1014135015007103</v>
       </c>
       <c r="B13">
-        <v>30.7863024997304</v>
+        <v>39.412905286025399</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>11.086540162263701</v>
+        <v>8.7621572729251902</v>
       </c>
       <c r="B14">
-        <v>25.445326306123899</v>
+        <v>33.079029576034401</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>13.221029926230001</v>
+        <v>9.1447771622803202</v>
       </c>
       <c r="B15">
-        <v>21.131214107971701</v>
+        <v>44.766931689715001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>14.674659992076499</v>
+        <v>10.4469455604497</v>
       </c>
       <c r="B16">
-        <v>18.4906121668234</v>
+        <v>26.6612902057627</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>17.1367203381796</v>
+        <v>12.512343717956799</v>
       </c>
       <c r="B17">
-        <v>14.403029956667201</v>
+        <v>21.6039587390826</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>19.714399637650999</v>
+        <v>13.9989445875703</v>
       </c>
       <c r="B18">
-        <v>11.1047685567921</v>
+        <v>17.604522871673002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>22.541189718014799</v>
+        <v>16.0173832403663</v>
       </c>
       <c r="B19">
-        <v>8.3869796419968594</v>
+        <v>14.4090697526594</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>25.3491937621916</v>
+        <v>18.560655288486</v>
       </c>
       <c r="B20">
-        <v>6.3121890520666097</v>
+        <v>11.212771153202899</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>27.954096173884299</v>
+        <v>21.262252697184699</v>
       </c>
       <c r="B21">
-        <v>4.82464428089542</v>
+        <v>8.7291844023060108</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>29.801427277065098</v>
+        <v>23.529018070784598</v>
       </c>
       <c r="B22">
-        <v>3.9120280447992202</v>
+        <v>6.5849134161323901</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>31.9381413554689</v>
+        <v>25.871948633781301</v>
       </c>
       <c r="B23">
-        <v>3.2112078285354699</v>
+        <v>5.47652739045009</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>33.701512883846597</v>
+        <v>29.072804382953301</v>
       </c>
       <c r="B24">
-        <v>2.60907253014076</v>
+        <v>4.4292995696422199</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>36.109098894319601</v>
+        <v>31.163733325723101</v>
       </c>
       <c r="B25">
-        <v>2.0893236627337899</v>
+        <v>3.28477154219238</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>38.606005256630603</v>
+        <v>32.326347885670899</v>
       </c>
       <c r="B26">
-        <v>1.6285273619312099</v>
+        <v>5.8424510213520398</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>41.527836641609703</v>
+        <v>33.654750654514302</v>
       </c>
       <c r="B27">
-        <v>1.2439783977274299</v>
+        <v>2.53303250117209</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>43.887672944765001</v>
+        <v>36.1977058896437</v>
       </c>
       <c r="B28">
-        <v>0.91311254106637496</v>
+        <v>2.0008160389890501</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>47.001826950049796</v>
+        <v>38.686720807110902</v>
       </c>
       <c r="B29">
-        <v>0.68584893320657903</v>
+        <v>1.55563377093876</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>49.267796913246798</v>
+        <v>41.599527334404002</v>
       </c>
       <c r="B30">
-        <v>0.49329822216580199</v>
+        <v>1.1893248134030301</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>54.477482995020203</v>
+        <v>43.613893514893697</v>
       </c>
       <c r="B31">
-        <v>0.34014980623567298</v>
+        <v>0.89250856625370201</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>56.462796987803998</v>
+        <v>46.2132871444987</v>
       </c>
       <c r="B32">
-        <v>0.25634284782254302</v>
+        <v>0.73494865583824998</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>60.8687897231612</v>
+        <v>48.5047571661094</v>
       </c>
       <c r="B33">
-        <v>0.18218110942808899</v>
+        <v>0.46831213076936401</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>63.268847012837703</v>
+        <v>48.2353987753513</v>
       </c>
       <c r="B34">
-        <v>0.121042157780367</v>
+        <v>0.604398687952172</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>64.940211589056005</v>
+        <v>54.494067774064099</v>
       </c>
       <c r="B35">
-        <v>8.8310602348460096E-2</v>
+        <v>0.32494650256065399</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>67.304352800524697</v>
+        <v>56.757968002344498</v>
       </c>
       <c r="B36">
-        <v>6.8446627050070499E-2</v>
+        <v>0.24617415358535499</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>71.051095493541098</v>
+        <v>58.675022645108903</v>
       </c>
       <c r="B37">
-        <v>5.1085742307097302E-2</v>
+        <v>0.44443288556222599</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>75.677116702132494</v>
+        <v>61.040589793358897</v>
       </c>
       <c r="B38">
-        <v>3.5553435166939901E-2</v>
+        <v>0.17473151875764001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>76.986691668114901</v>
+        <v>63.846555736272101</v>
       </c>
       <c r="B39">
-        <v>2.7748208041007999E-2</v>
+        <v>0.117323914081486</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>85.477650006688606</v>
+        <v>68.265341107002996</v>
       </c>
       <c r="B40">
-        <v>1.1330278663637601E-2</v>
+        <v>8.5775569736564306E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>91.994501206134501</v>
+        <v>66.246967750450395</v>
       </c>
       <c r="B41">
-        <v>4.8939678652236401E-3</v>
+        <v>0.44925200570586299</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>94.995048345824998</v>
+        <v>70.322036375775994</v>
       </c>
       <c r="B42">
-        <v>1.59983192549371E-3</v>
+        <v>6.3408360487477694E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>96.762959024491096</v>
+        <v>72.393505542767997</v>
       </c>
       <c r="B43">
-        <v>1.2925223368789099E-3</v>
+        <v>4.8351530876371299E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>113.70095782057599</v>
+        <v>78.051031204444399</v>
       </c>
       <c r="B44">
-        <v>1.04609218064063E-3</v>
+        <v>3.6640873828206903E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>136.04434132363201</v>
+        <v>81.358143409159098</v>
       </c>
       <c r="B45">
-        <v>7.9639939235247E-4</v>
+        <v>2.55262068377799E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>161.55212855826801</v>
+        <v>81.496142530730793</v>
       </c>
       <c r="B46">
-        <v>5.8304332030692995E-4</v>
+        <v>2.7112226828618301E-3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>182.12625823331899</v>
+        <v>80.896064482197104</v>
       </c>
       <c r="B47">
-        <v>4.6894811732143703E-4</v>
+        <v>1.8989171866098001E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>203.41223625609001</v>
+        <v>82.8777453045101</v>
       </c>
       <c r="B48">
-        <v>3.7614579180989899E-4</v>
+        <v>1.51663326967354E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>235.22511807625901</v>
+        <v>84.276648023166999</v>
       </c>
       <c r="B49">
-        <v>3.0040777950631999E-4</v>
+        <v>1.1474200878648901E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>269.85958334609302</v>
+        <v>86.643613588577693</v>
       </c>
       <c r="B50">
-        <v>2.35789198278995E-4</v>
+        <v>9.9672381548971595E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>318.39737104644303</v>
+        <v>86.496546609847698</v>
       </c>
       <c r="B51">
-        <v>1.9233740156918101E-4</v>
+        <v>7.9785609546122294E-2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>365.079639120965</v>
+        <v>86.346085833071001</v>
       </c>
       <c r="B52">
-        <v>1.5097291974243201E-4</v>
+        <v>6.3514624165424499E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>419.80451298070199</v>
+        <v>87.5875386177472</v>
       </c>
       <c r="B53">
-        <v>1.20692836258391E-4</v>
+        <v>8.7276918971913205E-3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>485.78503071000301</v>
+        <v>90.030859637044699</v>
       </c>
       <c r="B54" s="1">
-        <v>9.6382205947926695E-5</v>
+        <v>6.18393766969176E-3</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>561.79084593225696</v>
+        <v>87.003790957947203</v>
       </c>
       <c r="B55" s="1">
-        <v>7.7685492186039997E-5</v>
+        <v>5.0555110252974399E-2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>655.79953646961201</v>
+        <v>91.209509638601304</v>
       </c>
       <c r="B56" s="1">
-        <v>6.1429989804976003E-5</v>
+        <v>4.7180917555339798E-3</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>766.59880799493601</v>
+        <v>97.045815206610897</v>
       </c>
       <c r="B57" s="1">
-        <v>4.86741543837627E-5</v>
+        <v>3.5347882569146498E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>888.86973182429904</v>
+        <v>88.349552566529795</v>
       </c>
       <c r="B58" s="1">
-        <v>3.8940039623371102E-5</v>
+        <v>3.2763520924367198E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>1001.2753794142</v>
+        <v>95.123924984559594</v>
       </c>
       <c r="B59" s="1">
-        <v>3.0628958137867202E-5</v>
+        <v>3.49192757902548E-3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>1204.6832128313499</v>
+        <v>94.865130271119398</v>
       </c>
       <c r="B60" s="1">
-        <v>2.4835223316413401E-5</v>
+        <v>1.80038975524059E-3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1366.8453975648699</v>
+        <v>98.271826379985697</v>
       </c>
       <c r="B61" s="1">
-        <v>1.9762926960883999E-5</v>
+        <v>1.37821155828402E-3</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>1580.5658206133801</v>
+        <v>99.341778561223904</v>
       </c>
       <c r="B62" s="1">
-        <v>1.5702406017156599E-5</v>
+        <v>2.5206641425463399E-3</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>1800.1104189345899</v>
+        <v>110.57609466959001</v>
       </c>
       <c r="B63" s="1">
-        <v>1.38442756359114E-5</v>
+        <v>1.0810997293002401E-3</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>2150.68205073436</v>
+        <v>108.531296147633</v>
       </c>
       <c r="B64" s="1">
-        <v>9.9913835185145703E-6</v>
+        <v>3.4853114241845798E-2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>2508.4453869231302</v>
+        <v>109.047934348423</v>
       </c>
       <c r="B65" s="1">
-        <v>7.8082334896095392E-6</v>
+        <v>1.6594236197382301E-3</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>2928.79658559769</v>
+        <v>122.939263148932</v>
       </c>
       <c r="B66" s="1">
-        <v>6.1169326693710102E-6</v>
+        <v>8.1914637196573098E-4</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>3473.0750334785998</v>
+        <v>141.33065011476401</v>
       </c>
       <c r="B67" s="1">
-        <v>4.77977201231022E-6</v>
+        <v>6.4075855074308195E-4</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>4147.4340533139302</v>
+        <v>159.07563654518299</v>
       </c>
       <c r="B68" s="1">
-        <v>3.67233817295874E-6</v>
+        <v>5.1399535178800297E-4</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>4788.7301113032199</v>
+        <v>184.26929824817199</v>
       </c>
       <c r="B69" s="1">
-        <v>2.92129795750396E-6</v>
+        <v>4.1900055355496201E-4</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>5569.6668085525998</v>
+        <v>216.123753975559</v>
       </c>
       <c r="B70" s="1">
-        <v>2.3276475615925101E-6</v>
+        <v>3.2644129184313198E-4</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>6518.0657198635299</v>
+        <v>250.49950480627101</v>
       </c>
       <c r="B71" s="1">
-        <v>1.83474763079065E-6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2.5581057894239102E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>7950.1610284071303</v>
+        <v>250.905443557729</v>
       </c>
       <c r="B72" s="1">
-        <v>1.3081622749432499E-6</v>
+        <v>2.1042563118213101E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>303.07743952549203</v>
+      </c>
+      <c r="B73">
+        <v>2.0076997405015201E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>339.49576030262602</v>
+      </c>
+      <c r="B74">
+        <v>1.7256392386403899E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>395.62402844562899</v>
+      </c>
+      <c r="B75">
+        <v>1.2678615838915901E-4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>370.87013628711298</v>
+      </c>
+      <c r="B76">
+        <v>1.8231453403693199E-4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>461.78579671032497</v>
+      </c>
+      <c r="B77">
+        <v>9.8797488401080005E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>538.924100799793</v>
+      </c>
+      <c r="B78">
+        <v>7.7961525529283605E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>627.21338137340899</v>
+      </c>
+      <c r="B79">
+        <v>6.1822950516881098E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>734.10782031617305</v>
+      </c>
+      <c r="B80">
+        <v>4.8408666217356403E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>846.897692369315</v>
+      </c>
+      <c r="B81">
+        <v>4.0382334007166997E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>951.26593595622501</v>
+      </c>
+      <c r="B82">
+        <v>3.0406916100686101E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1098.9062216530699</v>
+      </c>
+      <c r="B83">
+        <v>2.6400590671502999E-5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1201.026131549</v>
+      </c>
+      <c r="B84">
+        <v>2.21750249519291E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1398.6619285531301</v>
+      </c>
+      <c r="B85">
+        <v>1.67807455661695E-5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1643.5524190533999</v>
+      </c>
+      <c r="B86">
+        <v>1.44636844949744E-5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1813.3746760596</v>
+      </c>
+      <c r="B87">
+        <v>1.19210692061932E-5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>2131.7633579895</v>
+      </c>
+      <c r="B88">
+        <v>9.4892639888764302E-6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>2482.9754241734599</v>
+      </c>
+      <c r="B89">
+        <v>7.4559063534511701E-6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>2887.5722612120899</v>
+      </c>
+      <c r="B90">
+        <v>5.8510619605561803E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>3423.3166876266901</v>
+      </c>
+      <c r="B91">
+        <v>4.5633272207078901E-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>4086.9464512763898</v>
+      </c>
+      <c r="B92">
+        <v>3.5061097179644399E-6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>4717.65946368408</v>
+      </c>
+      <c r="B93">
+        <v>2.7802954529325599E-6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>5485.7135259003899</v>
+      </c>
+      <c r="B94">
+        <v>2.21282709925747E-6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>6418.2891617462601</v>
+      </c>
+      <c r="B95">
+        <v>1.7444233816782701E-6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>7299.0485756717999</v>
+      </c>
+      <c r="B96">
+        <v>1.2781540600331E-6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>7947.6124466579804</v>
+      </c>
+      <c r="B97">
+        <v>1.3349797999698301E-6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>9078.6007991418501</v>
+      </c>
+      <c r="B98">
+        <v>1.1248959165915299E-6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>9459.4431575939907</v>
+      </c>
+      <c r="B99">
+        <v>1.6317509882533701E-6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>10050.6248573665</v>
+      </c>
+      <c r="B100" s="1">
+        <v>7.8568298476819795E-7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>10556.2744715643</v>
+      </c>
+      <c r="B101">
+        <v>1.21422512006453E-6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>11736.963222706399</v>
+      </c>
+      <c r="B102" s="1">
+        <v>7.1204060224130796E-7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>13106.7560347014</v>
+      </c>
+      <c r="B103" s="1">
+        <v>5.7904533682010705E-7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>15311.3134042727</v>
+      </c>
+      <c r="B104" s="1">
+        <v>4.6204223536916198E-7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>17802.546001398201</v>
+      </c>
+      <c r="B105" s="1">
+        <v>3.6367121301650998E-7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>20633.850060215202</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2.9135090582297602E-7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>23992.0141466803</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2.30483700714755E-7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>28144.987186210001</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1.8422259950331399E-7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>32726.027316800701</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1.45990928302693E-7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>36081.3550923855</v>
+      </c>
+      <c r="B110" s="1">
+        <v>9.6489569562621105E-8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>38151.687840322702</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1.2021627605778299E-7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>44237.405673204601</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1.01614257109751E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>